<commit_message>
fixed reindex problem for incremental update
</commit_message>
<xml_diff>
--- a/result/Result.xlsx
+++ b/result/Result.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:UM27"/>
+  <dimension ref="A1:UN27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2125,6 +2125,9 @@
       <c r="UM1" s="2" t="n">
         <v>44348</v>
       </c>
+      <c r="UN1" s="2" t="n">
+        <v>44349</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -3712,6 +3715,9 @@
       <c r="UM2" t="n">
         <v>3624.71</v>
       </c>
+      <c r="UN2" t="n">
+        <v>3597.14</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -5299,6 +5305,9 @@
       <c r="UM3" t="n">
         <v>15034.78</v>
       </c>
+      <c r="UN3" t="n">
+        <v>14857.91</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -6923,7 +6932,10 @@
       </c>
       <c r="UK4" t="inlineStr"/>
       <c r="UL4" t="inlineStr"/>
-      <c r="UM4" t="inlineStr"/>
+      <c r="UM4" t="n">
+        <v>4202.04</v>
+      </c>
+      <c r="UN4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -8548,7 +8560,10 @@
       </c>
       <c r="UK5" t="inlineStr"/>
       <c r="UL5" t="inlineStr"/>
-      <c r="UM5" t="inlineStr"/>
+      <c r="UM5" t="n">
+        <v>34576.3</v>
+      </c>
+      <c r="UN5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -10173,7 +10188,10 @@
       </c>
       <c r="UK6" t="inlineStr"/>
       <c r="UL6" t="inlineStr"/>
-      <c r="UM6" t="inlineStr"/>
+      <c r="UM6" t="n">
+        <v>13736.48</v>
+      </c>
+      <c r="UN6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -11775,6 +11793,9 @@
       <c r="UM7" t="n">
         <v>18258.93</v>
       </c>
+      <c r="UN7" t="n">
+        <v>18116.56</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -13380,6 +13401,9 @@
       <c r="UM8" t="n">
         <v>29493.12</v>
       </c>
+      <c r="UN8" t="n">
+        <v>29268.62</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -15009,7 +15033,10 @@
       <c r="UK9" t="inlineStr"/>
       <c r="UL9" t="inlineStr"/>
       <c r="UM9" t="n">
-        <v>17.11</v>
+        <v>17.9</v>
+      </c>
+      <c r="UN9" t="n">
+        <v>17.96</v>
       </c>
     </row>
     <row r="10">
@@ -16632,7 +16659,10 @@
         <v>15421.13</v>
       </c>
       <c r="UM10" t="n">
-        <v>15678.35</v>
+        <v>15567.36</v>
+      </c>
+      <c r="UN10" t="n">
+        <v>15586.55</v>
       </c>
     </row>
     <row r="11">
@@ -18257,7 +18287,10 @@
       <c r="UK11" t="inlineStr"/>
       <c r="UL11" t="inlineStr"/>
       <c r="UM11" t="n">
-        <v>7107.65</v>
+        <v>7080.46</v>
+      </c>
+      <c r="UN11" t="n">
+        <v>7091.7</v>
       </c>
     </row>
     <row r="12">
@@ -19892,6 +19925,9 @@
       <c r="UM12" t="n">
         <v>7142.6</v>
       </c>
+      <c r="UN12" t="n">
+        <v>7217.8</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -21531,7 +21567,10 @@
         <v>4039.46</v>
       </c>
       <c r="UM13" t="n">
-        <v>4098.9</v>
+        <v>4071.75</v>
+      </c>
+      <c r="UN13" t="n">
+        <v>4078.74</v>
       </c>
     </row>
     <row r="14">
@@ -23116,6 +23155,9 @@
       <c r="UM14" t="n">
         <v>3300.16</v>
       </c>
+      <c r="UN14" t="n">
+        <v>3243.02</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -24753,7 +24795,10 @@
         <v>6447.17</v>
       </c>
       <c r="UM15" t="n">
-        <v>6517.37</v>
+        <v>6489.4</v>
+      </c>
+      <c r="UN15" t="n">
+        <v>6508.29</v>
       </c>
     </row>
     <row r="16">
@@ -26428,7 +26473,10 @@
         <v>4.681</v>
       </c>
       <c r="UM16" t="n">
-        <v>4.6487</v>
+        <v>4.6523</v>
+      </c>
+      <c r="UN16" t="n">
+        <v>4.634</v>
       </c>
     </row>
     <row r="17">
@@ -28057,7 +28105,10 @@
       <c r="UK17" t="inlineStr"/>
       <c r="UL17" t="inlineStr"/>
       <c r="UM17" t="n">
-        <v>10238.25</v>
+        <v>10241</v>
+      </c>
+      <c r="UN17" t="n">
+        <v>10207.5</v>
       </c>
     </row>
     <row r="18">
@@ -29644,7 +29695,10 @@
         <v>73520</v>
       </c>
       <c r="UM18" t="n">
-        <v>73850</v>
+        <v>73540</v>
+      </c>
+      <c r="UN18" t="n">
+        <v>73420</v>
       </c>
     </row>
     <row r="19">
@@ -31319,7 +31373,10 @@
         <v>1911.15</v>
       </c>
       <c r="UM19" t="n">
-        <v>1910.8</v>
+        <v>1901.35</v>
+      </c>
+      <c r="UN19" t="n">
+        <v>1898.75</v>
       </c>
     </row>
     <row r="20">
@@ -32904,7 +32961,10 @@
         <v>392</v>
       </c>
       <c r="UM20" t="n">
-        <v>392.68</v>
+        <v>390.36</v>
+      </c>
+      <c r="UN20" t="n">
+        <v>386.1</v>
       </c>
     </row>
     <row r="21">
@@ -34534,6 +34594,9 @@
       <c r="UL21" t="inlineStr"/>
       <c r="UM21" t="n">
         <v>2482.75</v>
+      </c>
+      <c r="UN21" t="n">
+        <v>2475.25</v>
       </c>
     </row>
     <row r="22">
@@ -36118,6 +36181,9 @@
       <c r="UM22" t="n">
         <v>10.19</v>
       </c>
+      <c r="UN22" t="n">
+        <v>10.22</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
@@ -37699,6 +37765,9 @@
       <c r="UM23" t="n">
         <v>61.89</v>
       </c>
+      <c r="UN23" t="n">
+        <v>60.44</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
@@ -39313,7 +39382,10 @@
       <c r="UL24" t="n">
         <v>12450</v>
       </c>
-      <c r="UM24" t="inlineStr"/>
+      <c r="UM24" t="n">
+        <v>12457.09</v>
+      </c>
+      <c r="UN24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
@@ -40854,7 +40926,10 @@
       <c r="UL25" t="n">
         <v>3988</v>
       </c>
-      <c r="UM25" t="inlineStr"/>
+      <c r="UM25" t="n">
+        <v>4065</v>
+      </c>
+      <c r="UN25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
@@ -42395,7 +42470,10 @@
       <c r="UL26" t="n">
         <v>3695</v>
       </c>
-      <c r="UM26" t="inlineStr"/>
+      <c r="UM26" t="n">
+        <v>3720.5</v>
+      </c>
+      <c r="UN26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
@@ -43983,6 +44061,9 @@
       <c r="UM27" t="n">
         <v>23.92</v>
       </c>
+      <c r="UN27" t="n">
+        <v>23.88</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>